<commit_message>
finished a part of data analysis
</commit_message>
<xml_diff>
--- a/ET1_2Report/ExperimentalData/ExperimentalData.xlsx
+++ b/ET1_2Report/ExperimentalData/ExperimentalData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\ETLabR\ET1_2Report\ExperimentalData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5\5_WorkSpace\ETLabR\ET1_2Report\ExperimentalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A055E3FD-20A5-4AAD-AE41-EC5238AE4902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68F2335-3706-4435-BE9D-D0F66A81E312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{9DB6A0FF-80A9-463B-950A-20867DFE1CCE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{9DB6A0FF-80A9-463B-950A-20867DFE1CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="线性电阻元件的伏安特性" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>电压/V</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,6 +110,22 @@
   </si>
   <si>
     <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ix/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ix/mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测量值U2/V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算值U2/V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -108,6 +133,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="179" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,15 +176,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,30 +506,30 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -523,227 +555,227 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>0.96399999999999997</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>18.899999999999999</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.99399999999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>18.899999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.98199999999999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>8.2100000000000009</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.995</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>8.2100000000000009</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1929</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1.929</v>
+      </c>
+      <c r="B4" s="2">
         <v>37.83</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.988</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>37.78</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1.9630000000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>16.420000000000002</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>1.99</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>2.8940000000000001</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>56.8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2.9830000000000001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>55.9</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>2.9449999999999998</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>24.64</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>2.9849999999999999</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>24.65</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>3.8559999999999999</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>75.739999999999995</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>3.9769999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>75.86</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>3.9249999999999998</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>32.869999999999997</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>3.9809999999999999</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>32.89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>4.82</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>95.2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>4.97</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>95.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>4.91</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>41.12</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>4.9800000000000004</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>41.17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>5.78</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>113.8</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>5.96</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>114.7</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>5.89</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>49.4</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>5.97</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>49.48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>6.74</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>133.69999999999999</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>6.96</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>134.30000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>6.87</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>57.7</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>6.96</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>57.82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="2">
         <v>7.85</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>66.180000000000007</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>7.96</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>66.25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="2">
         <v>8.84</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>74.7</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>8.9600000000000009</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>74.790000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="2">
         <v>9.82</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>83.2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>9.9499999999999993</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>83.3</v>
       </c>
     </row>
@@ -767,9 +799,9 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -783,7 +815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.879</v>
       </c>
@@ -791,7 +823,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.8340000000000001</v>
       </c>
@@ -799,7 +831,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2.7770000000000001</v>
       </c>
@@ -807,7 +839,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.68</v>
       </c>
@@ -815,7 +847,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4.63</v>
       </c>
@@ -823,7 +855,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.6</v>
       </c>
@@ -831,7 +863,7 @@
         <v>50.4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6.55</v>
       </c>
@@ -839,7 +871,7 @@
         <v>55.3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7.57</v>
       </c>
@@ -847,7 +879,7 @@
         <v>59.4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8.5500000000000007</v>
       </c>
@@ -855,7 +887,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9.5399999999999991</v>
       </c>
@@ -863,7 +895,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10.56</v>
       </c>
@@ -871,7 +903,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11.52</v>
       </c>
@@ -887,148 +919,218 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E403CDD-D776-4F01-B4F2-5D62DC8868A0}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.58203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>300</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>5.9960000000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <f>B2/A2</f>
+        <v>1.9986666666666666E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>400</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>5.9960000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C17" si="0">B3/A3</f>
+        <v>1.4990000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>500</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>5.9960000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1992000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>600</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>5.9969999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>9.9950000000000004E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>700</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5.9969999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5671428571428565E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>800</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>5.9969999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>7.4962499999999994E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>900</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>6.6644444444444451E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>5.9979999999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2000</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.9989999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3000</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9993333333333334E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6000</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>9.9966666666666672E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9000</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>6.6644444444444444E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>200</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>4.1260000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0630000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>100</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>2.0640000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0640000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>90</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>1.857</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0633333333333333E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>60</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>1.24</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0666666666666667E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1039,15 +1141,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C23BD1E-7CF3-48AB-B049-7C9CEC02FCD6}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E14"/>
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1060,8 +1165,23 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -1074,8 +1194,27 @@
       <c r="E2">
         <v>0.313</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="3">
+        <f>B2/1000</f>
+        <v>1.21E-4</v>
+      </c>
+      <c r="I2" s="3">
+        <f>H2/G2</f>
+        <v>1.2099999999999999E-3</v>
+      </c>
+      <c r="K2">
+        <f>H2*1000</f>
+        <v>0.121</v>
+      </c>
+      <c r="L2">
+        <f>I2*1000</f>
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -1088,8 +1227,27 @@
       <c r="E3">
         <v>1.0429999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H12" si="0">B3/1000</f>
+        <v>2.2800000000000001E-4</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I25" si="1">H3/G3</f>
+        <v>1.14E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K25" si="2">H3*1000</f>
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L25" si="3">I3*1000</f>
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -1102,8 +1260,27 @@
       <c r="E4">
         <v>2.0859999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3199999999999999E-4</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1066666666666666E-3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>1.1066666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1116,8 +1293,27 @@
       <c r="E5">
         <v>3.13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.062E-3</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>1.062E-3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>1.0620000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1130,8 +1326,27 @@
       <c r="E6">
         <v>10.407</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>2.1080000000000001E-3</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.054E-3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>2.1080000000000001</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>1.054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1144,8 +1359,27 @@
       <c r="E7">
         <v>8.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1509999999999997E-3</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0503333333333332E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>3.1509999999999998</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>1.0503333333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1158,8 +1392,27 @@
       <c r="E8">
         <v>8.9499999999999993</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0468E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0468000000000001E-3</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>10.468</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>1.0468000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1172,8 +1425,27 @@
       <c r="E9">
         <v>11.442</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0930000000000001E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0465000000000001E-3</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>20.93</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>1.0465000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>30</v>
       </c>
@@ -1186,8 +1458,27 @@
       <c r="E10">
         <v>12.48</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1370999999999996E-2</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0456999999999999E-3</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>31.370999999999995</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>1.0456999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100</v>
       </c>
@@ -1200,8 +1491,27 @@
       <c r="E11">
         <v>13.526999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10438500000000001</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>1.04385E-3</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>104.38500000000001</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>1.0438499999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>200</v>
       </c>
@@ -1214,21 +1524,296 @@
       <c r="E12">
         <v>13.58</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>1.0449999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D13">
         <v>15000</v>
       </c>
       <c r="E13">
         <v>13.587999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>300</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.313</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0433333333333334E-3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>313</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>1.0433333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14">
         <v>16000</v>
       </c>
       <c r="E14">
         <v>13.6</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0429999999999999E-3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>1043</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>1.0429999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>2000</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2.0859999999999999</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0429999999999999E-3</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>2086</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>1.0429999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>3000</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3.13</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0433333333333334E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>3130</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>1.0433333333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="3">
+        <v>10.407</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0407000000000001E-3</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>10407</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>1.0407000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>8500</v>
+      </c>
+      <c r="H18" s="3">
+        <v>8.85</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0411764705882353E-3</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>8850</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>1.0411764705882351</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>8600</v>
+      </c>
+      <c r="H19" s="3">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0406976744186047E-3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>8950</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>1.0406976744186047</v>
+      </c>
+    </row>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>11000</v>
+      </c>
+      <c r="H20" s="3">
+        <v>11.442</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0401818181818181E-3</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>11442</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>1.0401818181818181</v>
+      </c>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>12000</v>
+      </c>
+      <c r="H21" s="3">
+        <v>12.48</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0400000000000001E-3</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>12480</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>13000</v>
+      </c>
+      <c r="H22" s="3">
+        <v>13.526999999999999</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0405384615384615E-3</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>13527</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>1.0405384615384614</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>14000</v>
+      </c>
+      <c r="H23" s="3">
+        <v>13.58</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="1"/>
+        <v>9.7000000000000005E-4</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>13580</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>0.97000000000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>15000</v>
+      </c>
+      <c r="H24" s="3">
+        <v>13.587999999999999</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="1"/>
+        <v>9.058666666666666E-4</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>13588</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>0.9058666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>16000</v>
+      </c>
+      <c r="H25" s="3">
+        <v>13.6</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="1"/>
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="2"/>
+        <v>13600</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>
@@ -1239,26 +1824,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B5CB78-7DC1-4849-A710-69B63B2B906F}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1268,8 +1856,12 @@
       <c r="C2">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>C2*A2</f>
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1279,8 +1871,12 @@
       <c r="C3">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">C3*A3</f>
+        <v>5.8999999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1290,8 +1886,12 @@
       <c r="C4">
         <v>5.84</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1300,6 +1900,10 @@
       </c>
       <c r="C5">
         <v>2.94</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>5.88</v>
       </c>
     </row>
   </sheetData>
@@ -1312,13 +1916,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4608B25E-A4B7-4414-BAB9-C0C1A42AF01F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1335,7 +1939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.3</v>
       </c>
@@ -1352,7 +1956,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.22</v>
       </c>
@@ -1369,7 +1973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.8</v>
       </c>
@@ -1383,7 +1987,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.37</v>
       </c>
@@ -1397,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13.6</v>
       </c>

</xml_diff>

<commit_message>
have done some data analysis for ET1_2
</commit_message>
<xml_diff>
--- a/ET1_2Report/ExperimentalData/ExperimentalData.xlsx
+++ b/ET1_2Report/ExperimentalData/ExperimentalData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5\5_WorkSpace\ETLabR\ET1_2Report\ExperimentalData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\ETLabR\ET1_2Report\ExperimentalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68F2335-3706-4435-BE9D-D0F66A81E312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362B9D28-3168-47D6-B77E-C91DE4AE96CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{9DB6A0FF-80A9-463B-950A-20867DFE1CCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="8" xr2:uid="{9DB6A0FF-80A9-463B-950A-20867DFE1CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="线性电阻元件的伏安特性" sheetId="1" r:id="rId1"/>
@@ -19,27 +19,21 @@
     <sheet name="电流源伏安特性" sheetId="4" r:id="rId4"/>
     <sheet name="CCVS-1" sheetId="5" r:id="rId5"/>
     <sheet name="CCVS-2" sheetId="6" r:id="rId6"/>
+    <sheet name="数据处理与分析" sheetId="8" r:id="rId7"/>
+    <sheet name="电压源受控" sheetId="9" r:id="rId8"/>
+    <sheet name="电流源受控" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
   <si>
     <t>电压/V</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,17 +121,57 @@
   <si>
     <t>计算值U2/V</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线性元件外接内接误差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实验</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>理论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内接：偏大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外接：偏小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对误差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阈值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电阻R/Ω</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ix/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="0.000"/>
-    <numFmt numFmtId="179" formatCode="0.000000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="178" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +187,27 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,26 +219,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,30 +567,30 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -555,227 +616,227 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>0.96399999999999997</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.99399999999999999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0.98199999999999998</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>8.2100000000000009</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0.995</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>8.2100000000000009</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1.929</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>37.83</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1.988</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>37.78</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1.9630000000000001</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>16.420000000000002</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>1.99</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2.8940000000000001</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>56.8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2.9830000000000001</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>55.9</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>2.9449999999999998</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>24.64</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>2.9849999999999999</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>24.65</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3.8559999999999999</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>75.739999999999995</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>3.9769999999999999</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>75.86</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>3.9249999999999998</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>32.869999999999997</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>3.9809999999999999</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>32.89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>4.82</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>95.2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>4.97</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>95.5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>4.91</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>41.12</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>4.9800000000000004</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>41.17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5.78</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>113.8</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>5.96</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>114.7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>5.89</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>49.4</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>5.97</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>49.48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>6.74</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>133.69999999999999</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>6.96</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>134.30000000000001</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>6.87</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>57.7</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>6.96</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>57.82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E10" s="2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
         <v>7.85</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.180000000000007</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>7.96</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>66.25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E11" s="2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
         <v>8.84</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>74.7</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>8.9600000000000009</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>74.790000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E12" s="2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
         <v>9.82</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>83.2</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>9.9499999999999993</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>83.3</v>
       </c>
     </row>
@@ -796,18 +857,21 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
       <c r="D1" t="s">
         <v>6</v>
       </c>
@@ -815,100 +879,148 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.879</v>
       </c>
       <c r="B2">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <f>1000*A2/B2</f>
+        <v>36.473029045643152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.8340000000000001</v>
       </c>
       <c r="B3">
         <v>29.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">1000*A3/B3</f>
+        <v>61.337792642140471</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.7770000000000001</v>
       </c>
       <c r="B4">
         <v>35.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>78.44632768361582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.68</v>
       </c>
       <c r="B5">
         <v>40.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>91.089108910891099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4.63</v>
       </c>
       <c r="B6">
         <v>45.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>101.75824175824175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.6</v>
       </c>
       <c r="B7">
         <v>50.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>111.11111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.55</v>
       </c>
       <c r="B8">
         <v>55.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>118.44484629294756</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7.57</v>
       </c>
       <c r="B9">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>127.44107744107744</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.5500000000000007</v>
       </c>
       <c r="B10">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>133.59375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.5399999999999991</v>
       </c>
       <c r="B11">
         <v>68.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>139.88269794721407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10.56</v>
       </c>
       <c r="B12">
         <v>71.599999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>147.48603351955308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11.52</v>
       </c>
       <c r="B13">
         <v>75.5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>152.58278145695365</v>
       </c>
     </row>
   </sheetData>
@@ -919,18 +1031,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E403CDD-D776-4F01-B4F2-5D62DC8868A0}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="E1" sqref="E1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -940,197 +1053,366 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>300</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>5.9960000000000004</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>B2/A2</f>
         <v>1.9986666666666666E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="G2" s="4">
+        <f>F2/E2</f>
+        <v>2.0666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>400</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>5.9960000000000004</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C17" si="0">B3/A3</f>
         <v>1.4990000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.857</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G17" si="1">F3/E3</f>
+        <v>2.0633333333333333E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>500</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5.9960000000000004</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>1.1992000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.0640000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>2.0640000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>600</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>5.9969999999999999</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>9.9950000000000004E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4.1260000000000003</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="1"/>
+        <v>2.0630000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>700</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>5.9969999999999999</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>8.5671428571428565E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>300</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5.9960000000000004</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>1.9986666666666666E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>800</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5.9969999999999999</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>7.4962499999999994E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>400</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5.9960000000000004</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>1.4990000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>900</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5.9980000000000002</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>6.6644444444444451E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>500</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5.9960000000000004</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1992000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1000</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>5.9980000000000002</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5.9979999999999999E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>600</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5.9969999999999999</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
+        <v>9.9950000000000004E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2000</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>5.9980000000000002</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>2.9989999999999999E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>700</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5.9969999999999999</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>8.5671428571428565E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3000</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>5.9980000000000002</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>1.9993333333333334E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>800</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5.9969999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>7.4962499999999994E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6000</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>5.9980000000000002</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>9.9966666666666672E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>900</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
+        <v>6.6644444444444451E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9000</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>5.9980000000000002</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>6.6644444444444444E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
+        <v>5.9979999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>200</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4.1260000000000003</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>2.0630000000000003E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>2000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="1"/>
+        <v>2.9989999999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>100</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>2.0640000000000001</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>2.0640000000000002E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>3000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>1.9993333333333334E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>90</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1.857</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>2.0633333333333333E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>6000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>9.9966666666666672E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>60</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>1.24</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>2.0666666666666667E-2</v>
+      </c>
+      <c r="E17">
+        <v>9000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5.9980000000000002</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="1"/>
+        <v>6.6644444444444444E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1144,15 +1426,15 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L25"/>
+      <selection activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1181,7 +1463,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -1197,11 +1479,11 @@
       <c r="G2">
         <v>0.1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <f>B2/1000</f>
         <v>1.21E-4</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <f>H2/G2</f>
         <v>1.2099999999999999E-3</v>
       </c>
@@ -1214,7 +1496,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -1230,11 +1512,11 @@
       <c r="G3">
         <v>0.2</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f t="shared" ref="H3:H12" si="0">B3/1000</f>
         <v>2.2800000000000001E-4</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <f t="shared" ref="I3:I25" si="1">H3/G3</f>
         <v>1.14E-3</v>
       </c>
@@ -1247,7 +1529,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -1263,11 +1545,11 @@
       <c r="G4">
         <v>0.3</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f t="shared" si="0"/>
         <v>3.3199999999999999E-4</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f t="shared" si="1"/>
         <v>1.1066666666666666E-3</v>
       </c>
@@ -1280,7 +1562,7 @@
         <v>1.1066666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1296,11 +1578,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f t="shared" si="0"/>
         <v>1.062E-3</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <f t="shared" si="1"/>
         <v>1.062E-3</v>
       </c>
@@ -1313,7 +1595,7 @@
         <v>1.0620000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1329,11 +1611,11 @@
       <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>2.1080000000000001E-3</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <f t="shared" si="1"/>
         <v>1.054E-3</v>
       </c>
@@ -1346,7 +1628,7 @@
         <v>1.054</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1362,11 +1644,11 @@
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>3.1509999999999997E-3</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f t="shared" si="1"/>
         <v>1.0503333333333332E-3</v>
       </c>
@@ -1379,7 +1661,7 @@
         <v>1.0503333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1395,11 +1677,11 @@
       <c r="G8">
         <v>10</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>1.0468E-2</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
         <v>1.0468000000000001E-3</v>
       </c>
@@ -1412,7 +1694,7 @@
         <v>1.0468000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1428,11 +1710,11 @@
       <c r="G9">
         <v>20</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>2.0930000000000001E-2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
         <v>1.0465000000000001E-3</v>
       </c>
@@ -1445,7 +1727,7 @@
         <v>1.0465000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>30</v>
       </c>
@@ -1461,11 +1743,11 @@
       <c r="G10">
         <v>30</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>3.1370999999999996E-2</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
         <v>1.0456999999999999E-3</v>
       </c>
@@ -1478,7 +1760,7 @@
         <v>1.0456999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100</v>
       </c>
@@ -1494,11 +1776,11 @@
       <c r="G11">
         <v>100</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <f t="shared" si="0"/>
         <v>0.10438500000000001</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
         <v>1.04385E-3</v>
       </c>
@@ -1511,7 +1793,7 @@
         <v>1.0438499999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>200</v>
       </c>
@@ -1527,11 +1809,11 @@
       <c r="G12">
         <v>200</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>0.20899999999999999</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <f t="shared" si="1"/>
         <v>1.0449999999999999E-3</v>
       </c>
@@ -1544,7 +1826,7 @@
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>15000</v>
       </c>
@@ -1554,10 +1836,10 @@
       <c r="G13">
         <v>300</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>0.313</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <f t="shared" si="1"/>
         <v>1.0433333333333334E-3</v>
       </c>
@@ -1570,7 +1852,7 @@
         <v>1.0433333333333334</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>16000</v>
       </c>
@@ -1580,10 +1862,10 @@
       <c r="G14">
         <v>1000</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>1.0429999999999999</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <f t="shared" si="1"/>
         <v>1.0429999999999999E-3</v>
       </c>
@@ -1596,14 +1878,14 @@
         <v>1.0429999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G15">
         <v>2000</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>2.0859999999999999</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <f t="shared" si="1"/>
         <v>1.0429999999999999E-3</v>
       </c>
@@ -1616,14 +1898,14 @@
         <v>1.0429999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G16">
         <v>3000</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>3.13</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <f t="shared" si="1"/>
         <v>1.0433333333333334E-3</v>
       </c>
@@ -1636,14 +1918,14 @@
         <v>1.0433333333333334</v>
       </c>
     </row>
-    <row r="17" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G17">
         <v>10000</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>10.407</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <f t="shared" si="1"/>
         <v>1.0407000000000001E-3</v>
       </c>
@@ -1656,14 +1938,14 @@
         <v>1.0407000000000002</v>
       </c>
     </row>
-    <row r="18" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G18">
         <v>8500</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>8.85</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <f t="shared" si="1"/>
         <v>1.0411764705882353E-3</v>
       </c>
@@ -1676,14 +1958,14 @@
         <v>1.0411764705882351</v>
       </c>
     </row>
-    <row r="19" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G19">
         <v>8600</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>8.9499999999999993</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <f t="shared" si="1"/>
         <v>1.0406976744186047E-3</v>
       </c>
@@ -1696,14 +1978,14 @@
         <v>1.0406976744186047</v>
       </c>
     </row>
-    <row r="20" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G20">
         <v>11000</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>11.442</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <f t="shared" si="1"/>
         <v>1.0401818181818181E-3</v>
       </c>
@@ -1716,14 +1998,14 @@
         <v>1.0401818181818181</v>
       </c>
     </row>
-    <row r="21" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>12000</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>12.48</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <f t="shared" si="1"/>
         <v>1.0400000000000001E-3</v>
       </c>
@@ -1736,14 +2018,14 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="22" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G22">
         <v>13000</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>13.526999999999999</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <f t="shared" si="1"/>
         <v>1.0405384615384615E-3</v>
       </c>
@@ -1756,14 +2038,14 @@
         <v>1.0405384615384614</v>
       </c>
     </row>
-    <row r="23" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G23">
         <v>14000</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>13.58</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <f t="shared" si="1"/>
         <v>9.7000000000000005E-4</v>
       </c>
@@ -1776,14 +2058,14 @@
         <v>0.97000000000000008</v>
       </c>
     </row>
-    <row r="24" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G24">
         <v>15000</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>13.587999999999999</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <f t="shared" si="1"/>
         <v>9.058666666666666E-4</v>
       </c>
@@ -1796,14 +2078,14 @@
         <v>0.9058666666666666</v>
       </c>
     </row>
-    <row r="25" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G25">
         <v>16000</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>13.6</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <f t="shared" si="1"/>
         <v>8.4999999999999995E-4</v>
       </c>
@@ -1826,13 +2108,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B5CB78-7DC1-4849-A710-69B63B2B906F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1846,7 +2128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1861,7 +2143,7 @@
         <v>5.88</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1876,7 +2158,7 @@
         <v>5.8999999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1891,7 +2173,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1920,9 +2202,9 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1939,7 +2221,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.3</v>
       </c>
@@ -1956,7 +2238,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.22</v>
       </c>
@@ -1973,7 +2255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.8</v>
       </c>
@@ -1987,7 +2269,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.37</v>
       </c>
@@ -2001,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13.6</v>
       </c>
@@ -2016,6 +2298,299 @@
       </c>
       <c r="E6">
         <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3031E6C8-98BB-4551-B38B-7AD0637C6B54}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>50.41</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>51.56</v>
+      </c>
+      <c r="D4">
+        <v>51</v>
+      </c>
+      <c r="E4">
+        <v>117.97</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="G4">
+        <v>119.36</v>
+      </c>
+      <c r="H4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6">
+        <f>(A4-B4)/B4</f>
+        <v>-1.1568627450980459E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="6">
+        <f>(C4-D4)/D4</f>
+        <v>1.098039215686279E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6">
+        <f>(E4-F4)/F4</f>
+        <v>-1.6916666666666677E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6">
+        <f>(G4-H4)/H4</f>
+        <v>-5.3333333333333384E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.14002800840280097</v>
+      </c>
+      <c r="B9">
+        <f>SQRT(51)</f>
+        <v>7.1414284285428504</v>
+      </c>
+      <c r="E9">
+        <f>SQRT(1/120)</f>
+        <v>9.1287092917527679E-2</v>
+      </c>
+      <c r="F9">
+        <f>SQRT(120)</f>
+        <v>10.954451150103322</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6204C4-4ED2-41AF-9801-4B97C7EDFA57}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>90</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.857</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.0640000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>200</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.1260000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>300</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.9960000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289E6DF2-5780-4B82-BB73-2656BAB70AEB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13000</v>
+      </c>
+      <c r="B2">
+        <v>1.0405384615384615E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>14000</v>
+      </c>
+      <c r="B3">
+        <v>9.7000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4">
+        <v>9.058666666666666E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>16000</v>
+      </c>
+      <c r="B5">
+        <v>8.4999999999999995E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>